<commit_message>
Update supplementary table 5 - add mTOR focusing analysis.
</commit_message>
<xml_diff>
--- a/supplementary tables/SupTable5/SupTable5.xlsx
+++ b/supplementary tables/SupTable5/SupTable5.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gongm/Documents/projects/LM_project/08312021_manuscript/TC_TFH_omics_analysis/supplementary tables/SupTable5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5FC6C7-AF98-0249-AFBD-B0578D6C4823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44027736-1A9A-424B-ABC1-B634A2B15672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{65A093C8-35B0-444D-AC1E-7710BDDAFDEB}"/>
+    <workbookView xWindow="-33160" yWindow="-13100" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{65A093C8-35B0-444D-AC1E-7710BDDAFDEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig3A-SupFig5A-RNA-seq" sheetId="1" r:id="rId1"/>
     <sheet name="Fig3B-FACS" sheetId="4" r:id="rId2"/>
     <sheet name="SupFig5B-GSEA" sheetId="3" r:id="rId3"/>
+    <sheet name="mTOR_activators" sheetId="5" r:id="rId4"/>
+    <sheet name="mTOR_suppresors" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="420">
   <si>
     <t>MouseSymbol</t>
   </si>
@@ -914,21 +916,12 @@
     <t>Tfh</t>
   </si>
   <si>
-    <t>HALLMARK_MTORC1_SIGNALING</t>
-  </si>
-  <si>
-    <t>tags=62%, list=28%, signal=86%</t>
-  </si>
-  <si>
     <t>tags=55%, list=16%, signal=65%</t>
   </si>
   <si>
     <t>Tn</t>
   </si>
   <si>
-    <t>tags=40%, list=20%, signal=49%</t>
-  </si>
-  <si>
     <t>BIOCARTA_MPR_PATHWAY</t>
   </si>
   <si>
@@ -1050,14 +1043,277 @@
   </si>
   <si>
     <t>tags=40%, list=6%, signal=43%</t>
+  </si>
+  <si>
+    <t>Zc3h12a</t>
+  </si>
+  <si>
+    <t>Zbtb11</t>
+  </si>
+  <si>
+    <t>Usp36</t>
+  </si>
+  <si>
+    <t>Smarcb1</t>
+  </si>
+  <si>
+    <t>Sf1</t>
+  </si>
+  <si>
+    <t>Sec31a</t>
+  </si>
+  <si>
+    <t>Rps6kb2</t>
+  </si>
+  <si>
+    <t>Rpap1</t>
+  </si>
+  <si>
+    <t>Rheb</t>
+  </si>
+  <si>
+    <t>Rbbp5</t>
+  </si>
+  <si>
+    <t>Prpf38b</t>
+  </si>
+  <si>
+    <t>Preb</t>
+  </si>
+  <si>
+    <t>Ppp3cb</t>
+  </si>
+  <si>
+    <t>Ppil4</t>
+  </si>
+  <si>
+    <t>Pnn</t>
+  </si>
+  <si>
+    <t>Pggt1b</t>
+  </si>
+  <si>
+    <t>Pdpk1</t>
+  </si>
+  <si>
+    <t>Pabpn1</t>
+  </si>
+  <si>
+    <t>Otud5</t>
+  </si>
+  <si>
+    <t>Nup85</t>
+  </si>
+  <si>
+    <t>Lcp2</t>
+  </si>
+  <si>
+    <t>Kmt2d</t>
+  </si>
+  <si>
+    <t>Kmt2b</t>
+  </si>
+  <si>
+    <t>Itgav</t>
+  </si>
+  <si>
+    <t>Ints1</t>
+  </si>
+  <si>
+    <t>Ino80</t>
+  </si>
+  <si>
+    <t>Huwe1</t>
+  </si>
+  <si>
+    <t>Gtf3c1</t>
+  </si>
+  <si>
+    <t>Gtf2a1</t>
+  </si>
+  <si>
+    <t>Gpn1</t>
+  </si>
+  <si>
+    <t>Fyb</t>
+  </si>
+  <si>
+    <t>Farsa</t>
+  </si>
+  <si>
+    <t>Exoc1</t>
+  </si>
+  <si>
+    <t>Eprs</t>
+  </si>
+  <si>
+    <t>Dhx16</t>
+  </si>
+  <si>
+    <t>Ddx23</t>
+  </si>
+  <si>
+    <t>Cul1</t>
+  </si>
+  <si>
+    <t>Cpsf6</t>
+  </si>
+  <si>
+    <t>Cpsf1</t>
+  </si>
+  <si>
+    <t>Cnot10</t>
+  </si>
+  <si>
+    <t>Ccdc174</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>Brd4</t>
+  </si>
+  <si>
+    <t>Bptf</t>
+  </si>
+  <si>
+    <t>Arid1a</t>
+  </si>
+  <si>
+    <t>Adnp</t>
+  </si>
+  <si>
+    <t>log2FC.pS6highvspS6low.p2.highstim</t>
+  </si>
+  <si>
+    <t>gene_symbol</t>
+  </si>
+  <si>
+    <t>Zdhhc15</t>
+  </si>
+  <si>
+    <t>Ywhaz</t>
+  </si>
+  <si>
+    <t>Wdr92</t>
+  </si>
+  <si>
+    <t>Wdr82</t>
+  </si>
+  <si>
+    <t>Vps4b</t>
+  </si>
+  <si>
+    <t>Uba1</t>
+  </si>
+  <si>
+    <t>Tram1</t>
+  </si>
+  <si>
+    <t>Tpt1</t>
+  </si>
+  <si>
+    <t>Timm21</t>
+  </si>
+  <si>
+    <t>Thap11</t>
+  </si>
+  <si>
+    <t>Tfdp1</t>
+  </si>
+  <si>
+    <t>Ssr2</t>
+  </si>
+  <si>
+    <t>Ssr1</t>
+  </si>
+  <si>
+    <t>Sit1</t>
+  </si>
+  <si>
+    <t>Sh3kbp1</t>
+  </si>
+  <si>
+    <t>Serbp1</t>
+  </si>
+  <si>
+    <t>Rbbp4</t>
+  </si>
+  <si>
+    <t>Ptpn1</t>
+  </si>
+  <si>
+    <t>Prox1</t>
+  </si>
+  <si>
+    <t>Otub1</t>
+  </si>
+  <si>
+    <t>Nck1</t>
+  </si>
+  <si>
+    <t>Naca</t>
+  </si>
+  <si>
+    <t>Myl6</t>
+  </si>
+  <si>
+    <t>Men1</t>
+  </si>
+  <si>
+    <t>Mapk3</t>
+  </si>
+  <si>
+    <t>Irgm2</t>
+  </si>
+  <si>
+    <t>Irf2</t>
+  </si>
+  <si>
+    <t>Ddit4</t>
+  </si>
+  <si>
+    <t>Coro1a</t>
+  </si>
+  <si>
+    <t>Cd5</t>
+  </si>
+  <si>
+    <t>Cd320</t>
+  </si>
+  <si>
+    <t>Cap1</t>
+  </si>
+  <si>
+    <t>Bcas3</t>
+  </si>
+  <si>
+    <t>Atg5</t>
+  </si>
+  <si>
+    <t>Atg12</t>
+  </si>
+  <si>
+    <t>Arhgap25</t>
+  </si>
+  <si>
+    <t># Related to Long et al.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1091,10 +1347,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12116,7 +12373,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M32"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13437,10 +13694,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37067B3A-9085-1246-AEBC-B1F8DEAEF2D5}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13520,34 +13777,34 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B3" t="s">
         <v>289</v>
       </c>
       <c r="C3">
-        <v>183</v>
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>-0.52566979999999996</v>
+        <v>-0.71066713000000004</v>
       </c>
       <c r="E3">
-        <v>-2.2513247000000001</v>
+        <v>-1.9766589999999999</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1.9255240000000001E-3</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="I3">
-        <v>3844</v>
+        <v>1658</v>
       </c>
       <c r="J3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="K3" t="s">
         <v>291</v>
@@ -13555,34 +13812,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B4" t="s">
         <v>289</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="D4">
-        <v>-0.71066713000000004</v>
+        <v>-0.41407406000000002</v>
       </c>
       <c r="E4">
-        <v>-1.9766589999999999</v>
+        <v>-1.7079728999999999</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1.9255240000000001E-3</v>
+        <v>3.0933505E-2</v>
       </c>
       <c r="H4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.158</v>
       </c>
       <c r="I4">
-        <v>1658</v>
+        <v>2479</v>
       </c>
       <c r="J4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K4" t="s">
         <v>291</v>
@@ -13590,34 +13847,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B5" t="s">
         <v>289</v>
       </c>
       <c r="C5">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D5">
-        <v>-0.41407406000000002</v>
+        <v>-0.35555061999999998</v>
       </c>
       <c r="E5">
-        <v>-1.7079728999999999</v>
+        <v>-1.4189304</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="G5">
-        <v>3.0933505E-2</v>
+        <v>0.19692183999999999</v>
       </c>
       <c r="H5">
-        <v>0.158</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="I5">
-        <v>2479</v>
+        <v>3083</v>
       </c>
       <c r="J5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="K5" t="s">
         <v>291</v>
@@ -13625,34 +13882,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
         <v>289</v>
       </c>
       <c r="C6">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>-0.35555061999999998</v>
+        <v>-0.46836056999999998</v>
       </c>
       <c r="E6">
-        <v>-1.4189304</v>
+        <v>-1.390317</v>
       </c>
       <c r="F6">
-        <v>1.8749999999999999E-2</v>
+        <v>8.6956519999999995E-2</v>
       </c>
       <c r="G6">
-        <v>0.19692183999999999</v>
+        <v>0.20906827</v>
       </c>
       <c r="H6">
-        <v>0.88800000000000001</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="I6">
-        <v>3083</v>
+        <v>1646</v>
       </c>
       <c r="J6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="K6" t="s">
         <v>291</v>
@@ -13660,31 +13917,31 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>289</v>
       </c>
       <c r="C7">
-        <v>24</v>
+        <v>246</v>
       </c>
       <c r="D7">
-        <v>-0.46836056999999998</v>
+        <v>-0.30827376000000001</v>
       </c>
       <c r="E7">
-        <v>-1.390317</v>
+        <v>-1.3723277</v>
       </c>
       <c r="F7">
-        <v>8.6956519999999995E-2</v>
+        <v>4.1152259999999996E-3</v>
       </c>
       <c r="G7">
-        <v>0.20906827</v>
+        <v>0.19782359999999999</v>
       </c>
       <c r="H7">
-        <v>0.93799999999999994</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="I7">
-        <v>1646</v>
+        <v>2079</v>
       </c>
       <c r="J7" t="s">
         <v>310</v>
@@ -13695,34 +13952,34 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>316</v>
       </c>
       <c r="B8" t="s">
         <v>289</v>
       </c>
       <c r="C8">
-        <v>246</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>-0.30827376000000001</v>
+        <v>-0.47982051999999997</v>
       </c>
       <c r="E8">
-        <v>-1.3723277</v>
+        <v>-1.3085290000000001</v>
       </c>
       <c r="F8">
-        <v>4.1152259999999996E-3</v>
+        <v>0.13412228000000001</v>
       </c>
       <c r="G8">
-        <v>0.19782359999999999</v>
+        <v>0.24713112000000001</v>
       </c>
       <c r="H8">
-        <v>0.95799999999999996</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="I8">
-        <v>2079</v>
+        <v>1532</v>
       </c>
       <c r="J8" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K8" t="s">
         <v>291</v>
@@ -13730,34 +13987,34 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B9" t="s">
         <v>289</v>
       </c>
       <c r="C9">
-        <v>16</v>
+        <v>225</v>
       </c>
       <c r="D9">
-        <v>-0.47982051999999997</v>
+        <v>0.28623873</v>
       </c>
       <c r="E9">
-        <v>-1.3085290000000001</v>
+        <v>1.2538482</v>
       </c>
       <c r="F9">
-        <v>0.13412228000000001</v>
+        <v>4.4088176999999999E-2</v>
       </c>
       <c r="G9">
-        <v>0.24713112000000001</v>
+        <v>0.21221836999999999</v>
       </c>
       <c r="H9">
-        <v>0.99199999999999999</v>
+        <v>0.998</v>
       </c>
       <c r="I9">
-        <v>1532</v>
+        <v>2891</v>
       </c>
       <c r="J9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K9" t="s">
         <v>291</v>
@@ -13765,34 +14022,34 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>321</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
         <v>289</v>
       </c>
       <c r="C10">
-        <v>225</v>
+        <v>112</v>
       </c>
       <c r="D10">
-        <v>0.28623873</v>
+        <v>0.31923970000000002</v>
       </c>
       <c r="E10">
-        <v>1.2538482</v>
+        <v>1.2739294999999999</v>
       </c>
       <c r="F10">
-        <v>4.4088176999999999E-2</v>
+        <v>5.3537282999999998E-2</v>
       </c>
       <c r="G10">
-        <v>0.21221836999999999</v>
+        <v>0.20150857</v>
       </c>
       <c r="H10">
-        <v>0.998</v>
+        <v>0.996</v>
       </c>
       <c r="I10">
-        <v>2891</v>
+        <v>2068</v>
       </c>
       <c r="J10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K10" t="s">
         <v>291</v>
@@ -13800,34 +14057,34 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>229</v>
+        <v>321</v>
       </c>
       <c r="B11" t="s">
         <v>289</v>
       </c>
       <c r="C11">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>0.31923970000000002</v>
+        <v>0.54599534999999999</v>
       </c>
       <c r="E11">
-        <v>1.2739294999999999</v>
+        <v>1.3327412999999999</v>
       </c>
       <c r="F11">
-        <v>5.3537282999999998E-2</v>
+        <v>0.14372470000000001</v>
       </c>
       <c r="G11">
-        <v>0.20150857</v>
+        <v>0.1817887</v>
       </c>
       <c r="H11">
-        <v>0.996</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="I11">
-        <v>2068</v>
+        <v>1647</v>
       </c>
       <c r="J11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K11" t="s">
         <v>291</v>
@@ -13835,34 +14092,34 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B12" t="s">
         <v>289</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D12">
-        <v>0.54599534999999999</v>
+        <v>0.43171394000000002</v>
       </c>
       <c r="E12">
-        <v>1.3327412999999999</v>
+        <v>1.4350337</v>
       </c>
       <c r="F12">
-        <v>0.14372470000000001</v>
+        <v>4.8582997000000003E-2</v>
       </c>
       <c r="G12">
-        <v>0.1817887</v>
+        <v>0.1078254</v>
       </c>
       <c r="H12">
-        <v>0.98399999999999999</v>
+        <v>0.872</v>
       </c>
       <c r="I12">
-        <v>1647</v>
+        <v>3592</v>
       </c>
       <c r="J12" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K12" t="s">
         <v>291</v>
@@ -13870,34 +14127,34 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>328</v>
+        <v>250</v>
       </c>
       <c r="B13" t="s">
         <v>289</v>
       </c>
       <c r="C13">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>0.43171394000000002</v>
+        <v>0.55957484000000002</v>
       </c>
       <c r="E13">
-        <v>1.4350337</v>
+        <v>1.5713044</v>
       </c>
       <c r="F13">
-        <v>4.8582997000000003E-2</v>
+        <v>2.8957528999999999E-2</v>
       </c>
       <c r="G13">
-        <v>0.1078254</v>
+        <v>5.9178254999999999E-2</v>
       </c>
       <c r="H13">
-        <v>0.872</v>
+        <v>0.498</v>
       </c>
       <c r="I13">
-        <v>3592</v>
+        <v>1279</v>
       </c>
       <c r="J13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K13" t="s">
         <v>291</v>
@@ -13905,34 +14162,34 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>250</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
         <v>289</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>0.55957484000000002</v>
+        <v>0.66388760000000002</v>
       </c>
       <c r="E14">
-        <v>1.5713044</v>
+        <v>1.6148473999999999</v>
       </c>
       <c r="F14">
-        <v>2.8957528999999999E-2</v>
+        <v>2.5742574000000001E-2</v>
       </c>
       <c r="G14">
-        <v>5.9178254999999999E-2</v>
+        <v>5.2489687E-2</v>
       </c>
       <c r="H14">
-        <v>0.498</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="I14">
-        <v>1279</v>
+        <v>1576</v>
       </c>
       <c r="J14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="K14" t="s">
         <v>291</v>
@@ -13940,34 +14197,34 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>329</v>
       </c>
       <c r="B15" t="s">
         <v>289</v>
       </c>
       <c r="C15">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D15">
-        <v>0.66388760000000002</v>
+        <v>0.52214660000000002</v>
       </c>
       <c r="E15">
-        <v>1.6148473999999999</v>
+        <v>1.8206496000000001</v>
       </c>
       <c r="F15">
-        <v>2.5742574000000001E-2</v>
+        <v>1.915709E-3</v>
       </c>
       <c r="G15">
-        <v>5.2489687E-2</v>
+        <v>7.6578540000000004E-3</v>
       </c>
       <c r="H15">
-        <v>0.39100000000000001</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="I15">
-        <v>1576</v>
+        <v>856</v>
       </c>
       <c r="J15" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K15" t="s">
         <v>291</v>
@@ -13975,34 +14232,34 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B16" t="s">
         <v>289</v>
       </c>
       <c r="C16">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>0.52214660000000002</v>
+        <v>0.78700930000000002</v>
       </c>
       <c r="E16">
-        <v>1.8206496000000001</v>
+        <v>1.8480573</v>
       </c>
       <c r="F16">
-        <v>1.915709E-3</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>7.6578540000000004E-3</v>
+        <v>6.5880729999999998E-3</v>
       </c>
       <c r="H16">
-        <v>4.4999999999999998E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="I16">
-        <v>856</v>
+        <v>847</v>
       </c>
       <c r="J16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K16" t="s">
         <v>291</v>
@@ -14010,533 +14267,1716 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="B17" t="s">
         <v>289</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="D17">
-        <v>0.78700930000000002</v>
+        <v>-0.61407940000000005</v>
       </c>
       <c r="E17">
-        <v>1.8480573</v>
+        <v>-2.1842847000000001</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>6.5880729999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>847</v>
+        <v>2003</v>
       </c>
       <c r="J17" t="s">
-        <v>337</v>
+        <v>292</v>
       </c>
       <c r="K17" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="B18" t="s">
         <v>289</v>
       </c>
       <c r="C18">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="D18">
-        <v>-0.61407940000000005</v>
+        <v>-0.43928440000000002</v>
       </c>
       <c r="E18">
-        <v>-2.1842847000000001</v>
+        <v>-1.7080097000000001</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>2.4331076E-2</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>0.156</v>
       </c>
       <c r="I18">
-        <v>2003</v>
+        <v>2333</v>
       </c>
       <c r="J18" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="K18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B19" t="s">
         <v>289</v>
       </c>
       <c r="C19">
-        <v>181</v>
+        <v>18</v>
       </c>
       <c r="D19">
-        <v>-0.49634193999999998</v>
+        <v>-0.62009619999999999</v>
       </c>
       <c r="E19">
-        <v>-2.0692987</v>
+        <v>-1.6751978000000001</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1.3972056E-2</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>2.7987972E-2</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>0.217</v>
       </c>
       <c r="I19">
-        <v>2464</v>
+        <v>1455</v>
       </c>
       <c r="J19" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B20" t="s">
         <v>289</v>
       </c>
       <c r="C20">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="D20">
-        <v>-0.43928440000000002</v>
+        <v>-0.40084666000000002</v>
       </c>
       <c r="E20">
-        <v>-1.7080097000000001</v>
+        <v>-1.5928990000000001</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>2.3094690000000002E-3</v>
       </c>
       <c r="G20">
-        <v>2.4331076E-2</v>
+        <v>4.1483632999999999E-2</v>
       </c>
       <c r="H20">
-        <v>0.156</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="I20">
-        <v>2333</v>
+        <v>1339</v>
       </c>
       <c r="J20" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>297</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>289</v>
       </c>
       <c r="C21">
-        <v>18</v>
+        <v>228</v>
       </c>
       <c r="D21">
-        <v>-0.62009619999999999</v>
+        <v>-0.36560163000000001</v>
       </c>
       <c r="E21">
-        <v>-1.6751978000000001</v>
+        <v>-1.5865978000000001</v>
       </c>
       <c r="F21">
-        <v>1.3972056E-2</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>2.7987972E-2</v>
+        <v>4.0914968000000003E-2</v>
       </c>
       <c r="H21">
-        <v>0.217</v>
+        <v>0.41</v>
       </c>
       <c r="I21">
-        <v>1455</v>
+        <v>1287</v>
       </c>
       <c r="J21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K21" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B22" t="s">
         <v>289</v>
       </c>
       <c r="C22">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D22">
-        <v>-0.40084666000000002</v>
+        <v>-0.35814124000000003</v>
       </c>
       <c r="E22">
-        <v>-1.5928990000000001</v>
+        <v>-1.4099553</v>
       </c>
       <c r="F22">
-        <v>2.3094690000000002E-3</v>
+        <v>8.6393089999999995E-3</v>
       </c>
       <c r="G22">
-        <v>4.1483632999999999E-2</v>
+        <v>0.13122833</v>
       </c>
       <c r="H22">
-        <v>0.39600000000000002</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="I22">
-        <v>1339</v>
+        <v>1153</v>
       </c>
       <c r="J22" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="K22" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>308</v>
       </c>
       <c r="B23" t="s">
         <v>289</v>
       </c>
       <c r="C23">
-        <v>228</v>
+        <v>161</v>
       </c>
       <c r="D23">
-        <v>-0.36560163000000001</v>
+        <v>-0.33346376</v>
       </c>
       <c r="E23">
-        <v>-1.5865978000000001</v>
+        <v>-1.3818706999999999</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1.3483146E-2</v>
       </c>
       <c r="G23">
-        <v>4.0914968000000003E-2</v>
+        <v>0.15221166999999999</v>
       </c>
       <c r="H23">
-        <v>0.41</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="I23">
-        <v>1287</v>
+        <v>2097</v>
       </c>
       <c r="J23" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="K23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>307</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
         <v>289</v>
       </c>
       <c r="C24">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="D24">
-        <v>-0.35814124000000003</v>
+        <v>-0.49806345000000002</v>
       </c>
       <c r="E24">
-        <v>-1.4099553</v>
+        <v>-1.3662888</v>
       </c>
       <c r="F24">
-        <v>8.6393089999999995E-3</v>
+        <v>9.3253970000000005E-2</v>
       </c>
       <c r="G24">
-        <v>0.13122833</v>
+        <v>0.15382630999999999</v>
       </c>
       <c r="H24">
-        <v>0.88700000000000001</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="I24">
-        <v>1153</v>
+        <v>3504</v>
       </c>
       <c r="J24" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="K24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B25" t="s">
         <v>289</v>
       </c>
       <c r="C25">
-        <v>161</v>
+        <v>35</v>
       </c>
       <c r="D25">
-        <v>-0.33346376</v>
+        <v>-0.42502372999999999</v>
       </c>
       <c r="E25">
-        <v>-1.3818706999999999</v>
+        <v>-1.3557113000000001</v>
       </c>
       <c r="F25">
-        <v>1.3483146E-2</v>
+        <v>7.8091110000000005E-2</v>
       </c>
       <c r="G25">
-        <v>0.15221166999999999</v>
+        <v>0.15270817</v>
       </c>
       <c r="H25">
-        <v>0.92600000000000005</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="I25">
-        <v>2097</v>
+        <v>1244</v>
       </c>
       <c r="J25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>314</v>
       </c>
       <c r="B26" t="s">
         <v>289</v>
       </c>
       <c r="C26">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D26">
-        <v>-0.49806345000000002</v>
+        <v>-0.43525708000000002</v>
       </c>
       <c r="E26">
-        <v>-1.3662888</v>
+        <v>-1.3216424</v>
       </c>
       <c r="F26">
-        <v>9.3253970000000005E-2</v>
+        <v>0.117256634</v>
       </c>
       <c r="G26">
-        <v>0.15382630999999999</v>
+        <v>0.17784572000000001</v>
       </c>
       <c r="H26">
-        <v>0.95099999999999996</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="I26">
-        <v>3504</v>
+        <v>2578</v>
       </c>
       <c r="J26" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K26" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="B27" t="s">
         <v>289</v>
       </c>
       <c r="C27">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="D27">
-        <v>-0.42502372999999999</v>
+        <v>0.37858861999999999</v>
       </c>
       <c r="E27">
-        <v>-1.3557113000000001</v>
+        <v>1.3678907</v>
       </c>
       <c r="F27">
-        <v>7.8091110000000005E-2</v>
+        <v>3.4482760000000001E-2</v>
       </c>
       <c r="G27">
-        <v>0.15270817</v>
+        <v>0.23656209</v>
       </c>
       <c r="H27">
-        <v>0.96199999999999997</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="I27">
-        <v>1244</v>
+        <v>2742</v>
       </c>
       <c r="J27" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="K27" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="B28" t="s">
         <v>289</v>
       </c>
       <c r="C28">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D28">
-        <v>-0.43525708000000002</v>
+        <v>0.48533595000000002</v>
       </c>
       <c r="E28">
-        <v>-1.3216424</v>
+        <v>1.6296253000000001</v>
       </c>
       <c r="F28">
-        <v>0.117256634</v>
+        <v>6.1224490000000003E-3</v>
       </c>
       <c r="G28">
-        <v>0.17784572000000001</v>
+        <v>7.1050520000000006E-2</v>
       </c>
       <c r="H28">
-        <v>0.98399999999999999</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="I28">
-        <v>2578</v>
+        <v>1071</v>
       </c>
       <c r="J28" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="K28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>326</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
         <v>289</v>
       </c>
       <c r="C29">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="D29">
-        <v>0.37858861999999999</v>
+        <v>0.69906690000000005</v>
       </c>
       <c r="E29">
-        <v>1.3678907</v>
+        <v>1.7167678</v>
       </c>
       <c r="F29">
-        <v>3.4482760000000001E-2</v>
+        <v>3.9682540000000001E-3</v>
       </c>
       <c r="G29">
-        <v>0.23656209</v>
+        <v>7.7048610000000003E-2</v>
       </c>
       <c r="H29">
-        <v>0.97099999999999997</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="I29">
-        <v>2742</v>
+        <v>1208</v>
       </c>
       <c r="J29" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="K29" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>332</v>
-      </c>
-      <c r="B30" t="s">
-        <v>289</v>
-      </c>
-      <c r="C30">
-        <v>47</v>
-      </c>
-      <c r="D30">
-        <v>0.48533595000000002</v>
-      </c>
-      <c r="E30">
-        <v>1.6296253000000001</v>
-      </c>
-      <c r="F30">
-        <v>6.1224490000000003E-3</v>
-      </c>
-      <c r="G30">
-        <v>7.1050520000000006E-2</v>
-      </c>
-      <c r="H30">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="I30">
-        <v>1071</v>
-      </c>
-      <c r="J30" t="s">
-        <v>333</v>
-      </c>
-      <c r="K30" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" t="s">
-        <v>289</v>
-      </c>
-      <c r="C31">
-        <v>12</v>
-      </c>
-      <c r="D31">
-        <v>0.69906690000000005</v>
-      </c>
-      <c r="E31">
-        <v>1.7167678</v>
-      </c>
-      <c r="F31">
-        <v>3.9682540000000001E-3</v>
-      </c>
-      <c r="G31">
-        <v>7.7048610000000003E-2</v>
-      </c>
-      <c r="H31">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="I31">
-        <v>1208</v>
-      </c>
-      <c r="J31" t="s">
-        <v>334</v>
-      </c>
-      <c r="K31" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
-    <sortCondition ref="K1:K31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K29">
+    <sortCondition ref="K1:K29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73701293-F6FE-F74D-9AD0-64C24982F748}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B3">
+        <v>-3.7451966240000001</v>
+      </c>
+      <c r="C3">
+        <v>0.56089361400000004</v>
+      </c>
+      <c r="D3">
+        <v>3.8038414E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4">
+        <v>-5.6325049839999997</v>
+      </c>
+      <c r="C4">
+        <v>0.39967077600000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.7600000000000008E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5">
+        <v>-1.118209614</v>
+      </c>
+      <c r="C5">
+        <v>0.30374520799999999</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.7800000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6">
+        <v>-2.372341198</v>
+      </c>
+      <c r="C6">
+        <v>0.46216184199999999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.3099999999999994E-11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>376</v>
+      </c>
+      <c r="B7">
+        <v>-1.59569581</v>
+      </c>
+      <c r="C7">
+        <v>0.21904057399999999</v>
+      </c>
+      <c r="D7">
+        <v>1.8162264000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8">
+        <v>-2.0139052340000001</v>
+      </c>
+      <c r="C8">
+        <v>0.21508549699999999</v>
+      </c>
+      <c r="D8">
+        <v>7.6744200000000004E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B9">
+        <v>-0.557733013</v>
+      </c>
+      <c r="C9">
+        <v>0.19671165700000001</v>
+      </c>
+      <c r="D9">
+        <v>2.8362830000000002E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B10">
+        <v>-4.1637187009999996</v>
+      </c>
+      <c r="C10">
+        <v>0.31497456499999998</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.5200000000000001E-11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>372</v>
+      </c>
+      <c r="B11">
+        <v>-1.203249214</v>
+      </c>
+      <c r="C11">
+        <v>0.27617750400000002</v>
+      </c>
+      <c r="D11">
+        <v>5.9194300000000005E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>371</v>
+      </c>
+      <c r="B12">
+        <v>-4.7804047199999999</v>
+      </c>
+      <c r="C12">
+        <v>0.118882127</v>
+      </c>
+      <c r="D12">
+        <v>1.5207909E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B13">
+        <v>-1.536879125</v>
+      </c>
+      <c r="C13">
+        <v>0.127647759</v>
+      </c>
+      <c r="D13">
+        <v>1.9367768E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>369</v>
+      </c>
+      <c r="B14">
+        <v>-2.6818680499999998</v>
+      </c>
+      <c r="C14">
+        <v>0.29923147999999999</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.65E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15">
+        <v>-4.0054228869999999</v>
+      </c>
+      <c r="C15">
+        <v>0.129400759</v>
+      </c>
+      <c r="D15">
+        <v>2.713249E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>367</v>
+      </c>
+      <c r="B16">
+        <v>-1.6549087870000001</v>
+      </c>
+      <c r="C16">
+        <v>0.405703125</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.2199999999999999E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>366</v>
+      </c>
+      <c r="B17">
+        <v>-2.7937841859999999</v>
+      </c>
+      <c r="C17">
+        <v>0.17408104599999999</v>
+      </c>
+      <c r="D17">
+        <v>2.4599993000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>365</v>
+      </c>
+      <c r="B18">
+        <v>-4.9274855579999999</v>
+      </c>
+      <c r="C18">
+        <v>0.24811204100000001</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.24E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>364</v>
+      </c>
+      <c r="B19">
+        <v>-2.702212287</v>
+      </c>
+      <c r="C19">
+        <v>0.20559026799999999</v>
+      </c>
+      <c r="D19">
+        <v>3.2346739999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>363</v>
+      </c>
+      <c r="B20">
+        <v>-3.9195394000000001E-2</v>
+      </c>
+      <c r="C20">
+        <v>0.16509378899999999</v>
+      </c>
+      <c r="D20">
+        <v>3.6684169000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21">
+        <v>-3.0639174169999999</v>
+      </c>
+      <c r="C21">
+        <v>0.14358184199999999</v>
+      </c>
+      <c r="D21">
+        <v>5.8329699999999998E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>361</v>
+      </c>
+      <c r="B22">
+        <v>-3.4131095990000002</v>
+      </c>
+      <c r="C22">
+        <v>0.32419803000000003</v>
+      </c>
+      <c r="D22">
+        <v>1.77617E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>360</v>
+      </c>
+      <c r="B23">
+        <v>-1.0614273599999999</v>
+      </c>
+      <c r="C23">
+        <v>0.219019829</v>
+      </c>
+      <c r="D23">
+        <v>4.3060720000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>359</v>
+      </c>
+      <c r="B24">
+        <v>-1.8528012030000001</v>
+      </c>
+      <c r="C24">
+        <v>0.31469611600000003</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.5200000000000001E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>358</v>
+      </c>
+      <c r="B25">
+        <v>-6.4136526319999998</v>
+      </c>
+      <c r="C25">
+        <v>0.31871363000000003</v>
+      </c>
+      <c r="D25">
+        <v>1.8841591000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26">
+        <v>-3.0317294769999998</v>
+      </c>
+      <c r="C26">
+        <v>0.31680377700000001</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8.3000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>357</v>
+      </c>
+      <c r="B27">
+        <v>-5.3156245560000004</v>
+      </c>
+      <c r="C27">
+        <v>0.34891856100000002</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8.6900000000000004E-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>356</v>
+      </c>
+      <c r="B28">
+        <v>-4.1238656459999996</v>
+      </c>
+      <c r="C28">
+        <v>0.55849501400000001</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1.2300000000000001E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>355</v>
+      </c>
+      <c r="B29">
+        <v>-5.9670076229999998</v>
+      </c>
+      <c r="C29">
+        <v>8.9090534999999998E-2</v>
+      </c>
+      <c r="D29">
+        <v>2.9302311000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>354</v>
+      </c>
+      <c r="B30">
+        <v>-2.0827540519999999</v>
+      </c>
+      <c r="C30">
+        <v>0.16337654900000001</v>
+      </c>
+      <c r="D30">
+        <v>1.6591576E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B31">
+        <v>-1.03347726</v>
+      </c>
+      <c r="C31">
+        <v>0.28069559199999999</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3.32E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>352</v>
+      </c>
+      <c r="B32">
+        <v>-2.37926254</v>
+      </c>
+      <c r="C32">
+        <v>0.49253785700000002</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7.1099999999999997E-6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>351</v>
+      </c>
+      <c r="B33">
+        <v>-2.03522062</v>
+      </c>
+      <c r="C33">
+        <v>0.25720646200000002</v>
+      </c>
+      <c r="D33">
+        <v>7.4932999999999998E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>350</v>
+      </c>
+      <c r="B34">
+        <v>-3.8467942129999999</v>
+      </c>
+      <c r="C34">
+        <v>0.20336673299999999</v>
+      </c>
+      <c r="D34">
+        <v>4.3316899999999998E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>349</v>
+      </c>
+      <c r="B35">
+        <v>-0.60378535700000002</v>
+      </c>
+      <c r="C35">
+        <v>0.35451451299999998</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3.9400000000000002E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>348</v>
+      </c>
+      <c r="B36">
+        <v>-1.4935089969999999</v>
+      </c>
+      <c r="C36">
+        <v>0.102999468</v>
+      </c>
+      <c r="D36">
+        <v>3.7913127999999997E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>347</v>
+      </c>
+      <c r="B37">
+        <v>-0.173115569</v>
+      </c>
+      <c r="C37">
+        <v>0.161522157</v>
+      </c>
+      <c r="D37">
+        <v>1.2528750000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>346</v>
+      </c>
+      <c r="B38">
+        <v>-2.3016200960000002</v>
+      </c>
+      <c r="C38">
+        <v>0.24821279500000001</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4.2200000000000003E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>345</v>
+      </c>
+      <c r="B39">
+        <v>-1.975697598</v>
+      </c>
+      <c r="C39">
+        <v>0.49274581000000001</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1.2699999999999999E-15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>344</v>
+      </c>
+      <c r="B40">
+        <v>-3.0952161660000002</v>
+      </c>
+      <c r="C40">
+        <v>0.16031061399999999</v>
+      </c>
+      <c r="D40">
+        <v>5.7413840000000004E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>343</v>
+      </c>
+      <c r="B41">
+        <v>-3.283602449</v>
+      </c>
+      <c r="C41">
+        <v>0.14352801100000001</v>
+      </c>
+      <c r="D41">
+        <v>3.6540317000000003E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>342</v>
+      </c>
+      <c r="B42">
+        <v>-1.8249241759999999</v>
+      </c>
+      <c r="C42">
+        <v>0.41479441299999997</v>
+      </c>
+      <c r="D42" s="1">
+        <v>6.8399999999999996E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>341</v>
+      </c>
+      <c r="B43">
+        <v>-3.474476535</v>
+      </c>
+      <c r="C43">
+        <v>0.279395491</v>
+      </c>
+      <c r="D43">
+        <v>5.8872500000000001E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>340</v>
+      </c>
+      <c r="B44">
+        <v>-4.534418176</v>
+      </c>
+      <c r="C44">
+        <v>9.9633548000000002E-2</v>
+      </c>
+      <c r="D44">
+        <v>4.4174434999999998E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>339</v>
+      </c>
+      <c r="B45">
+        <v>-1.967611097</v>
+      </c>
+      <c r="C45">
+        <v>0.358840936</v>
+      </c>
+      <c r="D45" s="1">
+        <v>3.9299999999999999E-7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>338</v>
+      </c>
+      <c r="B46">
+        <v>-3.190320045</v>
+      </c>
+      <c r="C46">
+        <v>0.18687741299999999</v>
+      </c>
+      <c r="D46">
+        <v>6.6465659999999996E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>337</v>
+      </c>
+      <c r="B47">
+        <v>-1.677908446</v>
+      </c>
+      <c r="C47">
+        <v>0.16977457900000001</v>
+      </c>
+      <c r="D47">
+        <v>9.0274020000000003E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>336</v>
+      </c>
+      <c r="B48">
+        <v>-2.1540921819999999</v>
+      </c>
+      <c r="C48">
+        <v>0.22373347099999999</v>
+      </c>
+      <c r="D48">
+        <v>6.8708400000000002E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>335</v>
+      </c>
+      <c r="B49">
+        <v>-6.0852793949999997</v>
+      </c>
+      <c r="C49">
+        <v>0.40062563600000001</v>
+      </c>
+      <c r="D49" s="1">
+        <v>3.4400000000000003E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11780CE-F798-3D43-8642-32213C298480}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="5" width="31.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3">
+        <v>6.5029311249999999</v>
+      </c>
+      <c r="C3">
+        <v>-0.28895510200000002</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.34E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B4">
+        <v>4.4458140630000003</v>
+      </c>
+      <c r="C4">
+        <v>-0.24503492399999999</v>
+      </c>
+      <c r="D4">
+        <v>8.9948299999999997E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B5">
+        <v>6.0392520770000004</v>
+      </c>
+      <c r="C5">
+        <v>-0.37073350700000002</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.2700000000000001E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B6">
+        <v>5.8864693910000003</v>
+      </c>
+      <c r="C6">
+        <v>-0.270419401</v>
+      </c>
+      <c r="D6">
+        <v>8.5285000000000005E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B7">
+        <v>3.415598932</v>
+      </c>
+      <c r="C7">
+        <v>-0.30458077900000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.9399999999999999E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8">
+        <v>6.6168079239999997</v>
+      </c>
+      <c r="C8">
+        <v>-0.44733269199999998</v>
+      </c>
+      <c r="D8">
+        <v>5.0697720000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>412</v>
+      </c>
+      <c r="B9">
+        <v>6.3890849989999996</v>
+      </c>
+      <c r="C9">
+        <v>-0.28337733700000001</v>
+      </c>
+      <c r="D9">
+        <v>9.1394399999999998E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10">
+        <v>7.1639128530000002</v>
+      </c>
+      <c r="C10">
+        <v>-0.50763166400000004</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6.5500000000000004E-17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>410</v>
+      </c>
+      <c r="B11">
+        <v>5.9800252479999996</v>
+      </c>
+      <c r="C11">
+        <v>-1.2585527809999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.0800000000000002E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>409</v>
+      </c>
+      <c r="B12">
+        <v>4.4936352260000003</v>
+      </c>
+      <c r="C12">
+        <v>-0.11816301799999999</v>
+      </c>
+      <c r="D12">
+        <v>4.5543484000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>408</v>
+      </c>
+      <c r="B13">
+        <v>5.9642437460000002</v>
+      </c>
+      <c r="C13">
+        <v>-0.33183570099999998</v>
+      </c>
+      <c r="D13">
+        <v>2.724466E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>407</v>
+      </c>
+      <c r="B14">
+        <v>4.4213791499999999</v>
+      </c>
+      <c r="C14">
+        <v>-0.23796425800000001</v>
+      </c>
+      <c r="D14">
+        <v>2.9883155000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>406</v>
+      </c>
+      <c r="B15">
+        <v>4.7831886270000004</v>
+      </c>
+      <c r="C15">
+        <v>-0.12425922</v>
+      </c>
+      <c r="D15">
+        <v>4.2842672999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>405</v>
+      </c>
+      <c r="B16">
+        <v>7.5767268960000003</v>
+      </c>
+      <c r="C16">
+        <v>-0.52972250200000004</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9.7000000000000003E-14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>404</v>
+      </c>
+      <c r="B17">
+        <v>2.2450072940000001</v>
+      </c>
+      <c r="C17">
+        <v>-0.46174455800000003</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3.1600000000000002E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>403</v>
+      </c>
+      <c r="B18">
+        <v>0.904199376</v>
+      </c>
+      <c r="C18">
+        <v>-0.29422387999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5.6100000000000002E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>402</v>
+      </c>
+      <c r="B19">
+        <v>5.9942025279999998</v>
+      </c>
+      <c r="C19">
+        <v>-0.129166437</v>
+      </c>
+      <c r="D19">
+        <v>3.1410624999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>401</v>
+      </c>
+      <c r="B20">
+        <v>5.3845497140000003</v>
+      </c>
+      <c r="C20">
+        <v>-2.884937436</v>
+      </c>
+      <c r="D20">
+        <v>1.5050490000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>400</v>
+      </c>
+      <c r="B21">
+        <v>7.58406001</v>
+      </c>
+      <c r="C21">
+        <v>-0.160296781</v>
+      </c>
+      <c r="D21">
+        <v>3.9538715000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>399</v>
+      </c>
+      <c r="B22">
+        <v>6.715394528</v>
+      </c>
+      <c r="C22">
+        <v>-0.152870796</v>
+      </c>
+      <c r="D22">
+        <v>2.7067649999999999E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>398</v>
+      </c>
+      <c r="B23">
+        <v>2.0661274380000001</v>
+      </c>
+      <c r="C23">
+        <v>-0.27294589600000002</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4.6600000000000005E-10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>397</v>
+      </c>
+      <c r="B24">
+        <v>6.5040543409999998</v>
+      </c>
+      <c r="C24">
+        <v>-0.18180449600000001</v>
+      </c>
+      <c r="D24">
+        <v>1.579083E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>396</v>
+      </c>
+      <c r="B25">
+        <v>3.8896425649999999</v>
+      </c>
+      <c r="C25">
+        <v>-0.55281192700000004</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.5100000000000001E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26">
+        <v>4.960795354</v>
+      </c>
+      <c r="C26">
+        <v>-0.63260837000000003</v>
+      </c>
+      <c r="D26">
+        <v>6.0907069999999999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>395</v>
+      </c>
+      <c r="B27">
+        <v>5.9795149900000002</v>
+      </c>
+      <c r="C27">
+        <v>-0.10813679700000001</v>
+      </c>
+      <c r="D27">
+        <v>2.2258267000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>394</v>
+      </c>
+      <c r="B28">
+        <v>5.9732915689999997</v>
+      </c>
+      <c r="C28">
+        <v>-0.38084853699999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1.2799999999999999E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>393</v>
+      </c>
+      <c r="B29">
+        <v>5.1576969879999996</v>
+      </c>
+      <c r="C29">
+        <v>-0.19650475000000001</v>
+      </c>
+      <c r="D29">
+        <v>3.6376089E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>392</v>
+      </c>
+      <c r="B30">
+        <v>1.2997004720000001</v>
+      </c>
+      <c r="C30">
+        <v>-0.43279353199999998</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31">
+        <v>4.4849937769999997</v>
+      </c>
+      <c r="C31">
+        <v>-0.35503438199999998</v>
+      </c>
+      <c r="D31">
+        <v>3.6924499999999998E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>390</v>
+      </c>
+      <c r="B32">
+        <v>5.7727906820000001</v>
+      </c>
+      <c r="C32">
+        <v>-0.41148826199999999</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.4100000000000001E-6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>389</v>
+      </c>
+      <c r="B33">
+        <v>5.9911448380000003</v>
+      </c>
+      <c r="C33">
+        <v>-0.35255885999999997</v>
+      </c>
+      <c r="D33" s="1">
+        <v>9.0700000000000007E-12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>388</v>
+      </c>
+      <c r="B34">
+        <v>1.8632081760000001</v>
+      </c>
+      <c r="C34">
+        <v>-0.20081339500000001</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3.2899999999999997E-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>387</v>
+      </c>
+      <c r="B35">
+        <v>0.38590934100000002</v>
+      </c>
+      <c r="C35">
+        <v>-0.18405509</v>
+      </c>
+      <c r="D35">
+        <v>1.692711E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>386</v>
+      </c>
+      <c r="B36">
+        <v>4.7941543920000003</v>
+      </c>
+      <c r="C36">
+        <v>-0.111832154</v>
+      </c>
+      <c r="D36">
+        <v>9.5755409999999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>385</v>
+      </c>
+      <c r="B37">
+        <v>5.0162659119999997</v>
+      </c>
+      <c r="C37">
+        <v>-0.388824858</v>
+      </c>
+      <c r="D37" s="1">
+        <v>9.5799999999999998E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>384</v>
+      </c>
+      <c r="B38">
+        <v>3.491232718</v>
+      </c>
+      <c r="C38">
+        <v>-0.34608963500000001</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.42E-10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>383</v>
+      </c>
+      <c r="B39">
+        <v>5.7582343590000002</v>
+      </c>
+      <c r="C39">
+        <v>-0.294098678</v>
+      </c>
+      <c r="D39">
+        <v>3.252146E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>